<commit_message>
added graphs for runtime and cutoff experiments
</commit_message>
<xml_diff>
--- a/pa2/runtimes.xlsx
+++ b/pa2/runtimes.xlsx
@@ -20,12 +20,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>Transpose Conventional</t>
   </si>
   <si>
     <t>Matrix Size</t>
+  </si>
+  <si>
+    <t>Strassen</t>
   </si>
   <si>
     <t>Strassen 4097</t>
@@ -126,6 +129,1389 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Strassen's Algorithm vs. Transpose Conventional</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Transpose Conventional</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>400.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>600.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>700.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>800.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>900.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1100.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1200.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1300.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1400.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1500.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1600.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1700.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1800.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1900.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2100.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2200.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2300.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2400.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2500.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2600.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2700.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2800.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2900.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3000.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3100.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3200.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>3300.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3400.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>3500.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3600.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>3700.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>3800.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>3900.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>4000.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>866.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6282.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22136.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>48767.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>92573.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>161525.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>256407.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>383990.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>526197.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>728522.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.049594E6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.397227E6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.804745E6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.264942E6</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.740827E6</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.409641E6</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.142773E6</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.832891E6</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5.607218E6</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6.384741E6</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>7.621612E6</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>8.829274E6</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>9.91283E6</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.132495E7</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.2696662E7</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.4420703E7</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.6080585E7</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.7970816E7</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.0021373E7</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.1643976E7</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2.4399262E7</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2.6853803E7</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2.9383052E7</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3.1968702E7</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>3.4530146E7</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3.815897E7</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>4.1322603E7</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>4.4684355E7</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>4.8450923E7</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>5.0170887E7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Strassen's</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>400.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>600.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>700.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>800.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>900.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1100.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1200.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1300.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1400.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1500.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1600.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1700.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1800.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1900.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2100.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2200.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2300.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2400.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2500.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2600.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2700.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2800.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2900.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3000.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3100.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3200.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>3300.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3400.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>3500.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3600.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>3700.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>3800.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>3900.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>4000.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>828.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6171.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20210.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>46338.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>89996.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>155527.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>244133.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>372252.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>522697.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>707002.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.017723E6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.333368E6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.731175E6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.167601E6</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.664953E6</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.299315E6</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.027726E6</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.67492E6</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5.447566E6</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6.166153E6</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>7.351584E6</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>8.42657E6</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>9.557286E6</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.0892655E7</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.2117729E7</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.485462E7</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.6143443E7</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.8357767E7</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.041674E7</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.173178E7</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2.4304082E7</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2.6939399E7</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2.9492673E7</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3.2112793E7</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>3.4327158E7</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3.8931702E7</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>4.0955109E7</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>4.4334295E7</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>4.6776635E7</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>4.9583174E7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="631089320"/>
+        <c:axId val="631092408"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="631089320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="631092408"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="631092408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time in microseconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="631089320"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Performance of Strassen under different cutoffs</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Time to compute 4097x4097 mult. in microseconds</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet2!$A$2:$A$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>400.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>600.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>700.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>800.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>900.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1100.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1200.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1300.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1400.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1500.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1600.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1700.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1800.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1900.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2100.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2200.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2300.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2400.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2500.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2600.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2700.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2800.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2900.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3000.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3100.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3200.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>3300.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3400.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>3500.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3600.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>3700.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>3800.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>3900.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>4000.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$2:$B$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>4.0410344E7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.4323195E7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.3698865E7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.3721663E7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.4169796E7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.6203664E7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.5920371E7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.4855861E7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.5544991E7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.6587714E7</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.211639E7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.1806098E7</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.1841326E7</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.0694236E7</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.1896986E7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4.2278166E7</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.1311758E7</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.2436252E7</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4.1646366E7</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4.1483843E7</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4.7754704E7</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4.7813122E7</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4.8280666E7</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4.8503332E7</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>4.789562E7</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>5.049363E7</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>5.1805148E7</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>5.1537311E7</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>5.1938176E7</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>5.1555036E7</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>5.2021853E7</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>5.1772267E7</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>5.1687864E7</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>5.2029409E7</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>5.1864167E7</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>5.175029E7</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>5.2105804E7</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>5.1843233E7</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>5.2156258E7</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>4.7660819E7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="780268184"/>
+        <c:axId val="780271272"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="780268184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Size at which algortihm</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> sqitches to conventional multiplication</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="780271272"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="780271272"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time to compute 4097x4097 mult.</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> in microseconds</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="780268184"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Performance of Strassen under</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> different cutoff</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Runtime of Strassen's on 4097x4097 matrix</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet2!$G$2:$G$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>56.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$R$2:$R$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5.48396358E7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.84182948E7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.7713751E7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.97325914E7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.78691987E7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="705736600"/>
+        <c:axId val="705807400"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="705736600"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Size</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> at which algorithm switches to conventional multiplication</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="705807400"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="705807400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time to compute 4097 x 4097 mult. in microseconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="705736600"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>736600</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -450,344 +1836,468 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B41"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B31" sqref="B31:C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>100</v>
       </c>
       <c r="B2">
         <v>866</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>200</v>
       </c>
       <c r="B3">
         <v>6282</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3">
+        <v>6171</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>300</v>
       </c>
       <c r="B4">
         <v>22136</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4">
+        <v>20210</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>400</v>
       </c>
       <c r="B5">
         <v>48767</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5">
+        <v>46338</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6">
         <v>500</v>
       </c>
       <c r="B6">
         <v>92573</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="C6">
+        <v>89996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7">
         <v>600</v>
       </c>
       <c r="B7">
         <v>161525</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="C7">
+        <v>155527</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8">
         <v>700</v>
       </c>
       <c r="B8">
         <v>256407</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="C8">
+        <v>244133</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9">
         <v>800</v>
       </c>
       <c r="B9">
         <v>383990</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="C9">
+        <v>372252</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10">
         <v>900</v>
       </c>
       <c r="B10">
         <v>526197</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
+      <c r="C10">
+        <v>522697</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11">
         <v>1000</v>
       </c>
       <c r="B11">
         <v>728522</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
+      <c r="C11">
+        <v>707002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12">
         <v>1100</v>
       </c>
       <c r="B12">
         <v>1049594</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
+      <c r="C12">
+        <v>1017723</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13">
         <v>1200</v>
       </c>
       <c r="B13">
         <v>1397227</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
+      <c r="C13">
+        <v>1333368</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14">
         <v>1300</v>
       </c>
       <c r="B14">
         <v>1804745</v>
       </c>
-    </row>
-    <row r="15" spans="1:2">
+      <c r="C14">
+        <v>1731175</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15">
         <v>1400</v>
       </c>
       <c r="B15">
         <v>2264942</v>
       </c>
-    </row>
-    <row r="16" spans="1:2">
+      <c r="C15">
+        <v>2167601</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16">
         <v>1500</v>
       </c>
       <c r="B16">
         <v>2740827</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="C16">
+        <v>2664953</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17">
         <v>1600</v>
       </c>
       <c r="B17">
         <v>3409641</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="C17">
+        <v>3299315</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18">
         <v>1700</v>
       </c>
       <c r="B18">
         <v>4142773</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
+      <c r="C18">
+        <v>4027726</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19">
         <v>1800</v>
       </c>
       <c r="B19">
         <v>4832891</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
+      <c r="C19">
+        <v>4674920</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20">
         <v>1900</v>
       </c>
       <c r="B20">
         <v>5607218</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
+      <c r="C20">
+        <v>5447566</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21">
         <v>2000</v>
       </c>
       <c r="B21">
         <v>6384741</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
+      <c r="C21">
+        <v>6166153</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22">
         <v>2100</v>
       </c>
       <c r="B22">
         <v>7621612</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
+      <c r="C22">
+        <v>7351584</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23">
         <v>2200</v>
       </c>
       <c r="B23">
         <v>8829274</v>
       </c>
-    </row>
-    <row r="24" spans="1:2">
+      <c r="C23">
+        <v>8426570</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24">
         <v>2300</v>
       </c>
       <c r="B24">
         <v>9912830</v>
       </c>
-    </row>
-    <row r="25" spans="1:2">
+      <c r="C24">
+        <v>9557286</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25">
         <v>2400</v>
       </c>
       <c r="B25">
         <v>11324950</v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
+      <c r="C25">
+        <v>10892655</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
       <c r="A26">
         <v>2500</v>
       </c>
       <c r="B26">
         <v>12696662</v>
       </c>
-    </row>
-    <row r="27" spans="1:2">
+      <c r="C26">
+        <v>12117729</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27">
         <v>2600</v>
       </c>
       <c r="B27">
         <v>14420703</v>
       </c>
-    </row>
-    <row r="28" spans="1:2">
+      <c r="C27">
+        <v>14854620</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
       <c r="A28">
         <v>2700</v>
       </c>
       <c r="B28">
         <v>16080585</v>
       </c>
-    </row>
-    <row r="29" spans="1:2">
+      <c r="C28">
+        <v>16143443</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29">
         <v>2800</v>
       </c>
       <c r="B29">
         <v>17970816</v>
       </c>
-    </row>
-    <row r="30" spans="1:2">
+      <c r="C29">
+        <v>18357767</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
       <c r="A30">
         <v>2900</v>
       </c>
       <c r="B30">
         <v>20021373</v>
       </c>
-    </row>
-    <row r="31" spans="1:2">
+      <c r="C30">
+        <v>20416740</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
       <c r="A31">
         <v>3000</v>
       </c>
       <c r="B31">
         <v>21643976</v>
       </c>
-    </row>
-    <row r="32" spans="1:2">
+      <c r="C31">
+        <v>21731780</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
       <c r="A32">
         <v>3100</v>
       </c>
       <c r="B32">
         <v>24399262</v>
       </c>
-    </row>
-    <row r="33" spans="1:2">
+      <c r="C32">
+        <v>24304082</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
       <c r="A33">
         <v>3200</v>
       </c>
       <c r="B33">
         <v>26853803</v>
       </c>
-    </row>
-    <row r="34" spans="1:2">
+      <c r="C33">
+        <v>26939399</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
       <c r="A34">
         <v>3300</v>
       </c>
       <c r="B34">
         <v>29383052</v>
       </c>
-    </row>
-    <row r="35" spans="1:2">
+      <c r="C34">
+        <v>29492673</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
       <c r="A35">
         <v>3400</v>
       </c>
       <c r="B35">
         <v>31968702</v>
       </c>
-    </row>
-    <row r="36" spans="1:2">
+      <c r="C35">
+        <v>32112793</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
       <c r="A36">
         <v>3500</v>
       </c>
       <c r="B36">
         <v>34530146</v>
       </c>
-    </row>
-    <row r="37" spans="1:2">
+      <c r="C36">
+        <v>34327158</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
       <c r="A37">
         <v>3600</v>
       </c>
       <c r="B37">
         <v>38158970</v>
       </c>
-    </row>
-    <row r="38" spans="1:2">
+      <c r="C37">
+        <v>38931702</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
       <c r="A38">
         <v>3700</v>
       </c>
       <c r="B38">
         <v>41322603</v>
       </c>
-    </row>
-    <row r="39" spans="1:2">
+      <c r="C38">
+        <v>40955109</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
       <c r="A39">
         <v>3800</v>
       </c>
       <c r="B39">
         <v>44684355</v>
       </c>
-    </row>
-    <row r="40" spans="1:2">
+      <c r="C39">
+        <v>44334295</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
       <c r="A40">
         <v>3900</v>
       </c>
       <c r="B40">
         <v>48450923</v>
       </c>
-    </row>
-    <row r="41" spans="1:2">
+      <c r="C40">
+        <v>46776635</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
       <c r="A41">
         <v>4000</v>
       </c>
       <c r="B41">
         <v>50170887</v>
       </c>
+      <c r="C41">
+        <v>49583174</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -801,59 +2311,59 @@
   <dimension ref="A1:R41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7"/>
+      <selection activeCell="R2" sqref="R2:R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
       <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
       <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" t="s">
-        <v>2</v>
-      </c>
       <c r="I1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="N1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="O1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="P1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="Q1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="R1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:18">
@@ -1472,6 +2982,7 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
fixed arror in chart
</commit_message>
<xml_diff>
--- a/pa2/runtimes.xlsx
+++ b/pa2/runtimes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -584,124 +584,124 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="40"/>
                 <c:pt idx="0">
-                  <c:v>828.0</c:v>
+                  <c:v>1668.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6171.0</c:v>
+                  <c:v>12747.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20210.0</c:v>
+                  <c:v>93643.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>46338.0</c:v>
+                  <c:v>93590.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>89996.0</c:v>
+                  <c:v>93900.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>155527.0</c:v>
+                  <c:v>674354.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>244133.0</c:v>
+                  <c:v>669063.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>372252.0</c:v>
+                  <c:v>671395.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>522697.0</c:v>
+                  <c:v>672281.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>707002.0</c:v>
+                  <c:v>667612.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.017723E6</c:v>
+                  <c:v>4.74879E6</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.333368E6</c:v>
+                  <c:v>4.725772E6</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.731175E6</c:v>
+                  <c:v>4.715679E6</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.167601E6</c:v>
+                  <c:v>4.799687E6</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.664953E6</c:v>
+                  <c:v>4.765063E6</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.299315E6</c:v>
+                  <c:v>4.82891E6</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4.027726E6</c:v>
+                  <c:v>4.788924E6</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4.67492E6</c:v>
+                  <c:v>4.766968E6</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5.447566E6</c:v>
+                  <c:v>4.741763E6</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>6.166153E6</c:v>
+                  <c:v>4.731089E6</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>7.351584E6</c:v>
+                  <c:v>3.3662863E7</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>8.42657E6</c:v>
+                  <c:v>3.3275755E7</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>9.557286E6</c:v>
+                  <c:v>3.3755787E7</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1.0892655E7</c:v>
+                  <c:v>3.4315809E7</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.2117729E7</c:v>
+                  <c:v>3.4640412E7</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1.485462E7</c:v>
+                  <c:v>3.530582E7</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1.6143443E7</c:v>
+                  <c:v>3.4554925E7</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1.8357767E7</c:v>
+                  <c:v>3.4137404E7</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.041674E7</c:v>
+                  <c:v>3.4632744E7</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2.173178E7</c:v>
+                  <c:v>3.4763739E7</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2.4304082E7</c:v>
+                  <c:v>3.4131775E7</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2.6939399E7</c:v>
+                  <c:v>3.4729742E7</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2.9492673E7</c:v>
+                  <c:v>3.4495461E7</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>3.2112793E7</c:v>
+                  <c:v>3.5604467E7</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>3.4327158E7</c:v>
+                  <c:v>3.7001781E7</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>3.8931702E7</c:v>
+                  <c:v>3.5034148E7</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>4.0955109E7</c:v>
+                  <c:v>3.4622546E7</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>4.4334295E7</c:v>
+                  <c:v>3.4796305E7</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>4.6776635E7</c:v>
+                  <c:v>3.4311252E7</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>4.9583174E7</c:v>
+                  <c:v>3.5468807E7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1838,8 +1838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31:C41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1863,7 +1863,7 @@
         <v>866</v>
       </c>
       <c r="C2">
-        <v>828</v>
+        <v>1668</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1874,7 +1874,7 @@
         <v>6282</v>
       </c>
       <c r="C3">
-        <v>6171</v>
+        <v>12747</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1885,7 +1885,7 @@
         <v>22136</v>
       </c>
       <c r="C4">
-        <v>20210</v>
+        <v>93643</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1896,7 +1896,7 @@
         <v>48767</v>
       </c>
       <c r="C5">
-        <v>46338</v>
+        <v>93590</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1907,7 +1907,7 @@
         <v>92573</v>
       </c>
       <c r="C6">
-        <v>89996</v>
+        <v>93900</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1918,7 +1918,7 @@
         <v>161525</v>
       </c>
       <c r="C7">
-        <v>155527</v>
+        <v>674354</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1929,7 +1929,7 @@
         <v>256407</v>
       </c>
       <c r="C8">
-        <v>244133</v>
+        <v>669063</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1940,7 +1940,7 @@
         <v>383990</v>
       </c>
       <c r="C9">
-        <v>372252</v>
+        <v>671395</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1951,7 +1951,7 @@
         <v>526197</v>
       </c>
       <c r="C10">
-        <v>522697</v>
+        <v>672281</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1962,7 +1962,7 @@
         <v>728522</v>
       </c>
       <c r="C11">
-        <v>707002</v>
+        <v>667612</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -1973,7 +1973,7 @@
         <v>1049594</v>
       </c>
       <c r="C12">
-        <v>1017723</v>
+        <v>4748790</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -1984,7 +1984,7 @@
         <v>1397227</v>
       </c>
       <c r="C13">
-        <v>1333368</v>
+        <v>4725772</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -1995,7 +1995,7 @@
         <v>1804745</v>
       </c>
       <c r="C14">
-        <v>1731175</v>
+        <v>4715679</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -2006,7 +2006,7 @@
         <v>2264942</v>
       </c>
       <c r="C15">
-        <v>2167601</v>
+        <v>4799687</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -2017,7 +2017,7 @@
         <v>2740827</v>
       </c>
       <c r="C16">
-        <v>2664953</v>
+        <v>4765063</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -2028,7 +2028,7 @@
         <v>3409641</v>
       </c>
       <c r="C17">
-        <v>3299315</v>
+        <v>4828910</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -2039,7 +2039,7 @@
         <v>4142773</v>
       </c>
       <c r="C18">
-        <v>4027726</v>
+        <v>4788924</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -2050,7 +2050,7 @@
         <v>4832891</v>
       </c>
       <c r="C19">
-        <v>4674920</v>
+        <v>4766968</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -2061,7 +2061,7 @@
         <v>5607218</v>
       </c>
       <c r="C20">
-        <v>5447566</v>
+        <v>4741763</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -2072,7 +2072,7 @@
         <v>6384741</v>
       </c>
       <c r="C21">
-        <v>6166153</v>
+        <v>4731089</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -2083,7 +2083,7 @@
         <v>7621612</v>
       </c>
       <c r="C22">
-        <v>7351584</v>
+        <v>33662863</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -2094,7 +2094,7 @@
         <v>8829274</v>
       </c>
       <c r="C23">
-        <v>8426570</v>
+        <v>33275755</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -2105,7 +2105,7 @@
         <v>9912830</v>
       </c>
       <c r="C24">
-        <v>9557286</v>
+        <v>33755787</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -2116,7 +2116,7 @@
         <v>11324950</v>
       </c>
       <c r="C25">
-        <v>10892655</v>
+        <v>34315809</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -2127,7 +2127,7 @@
         <v>12696662</v>
       </c>
       <c r="C26">
-        <v>12117729</v>
+        <v>34640412</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -2138,7 +2138,7 @@
         <v>14420703</v>
       </c>
       <c r="C27">
-        <v>14854620</v>
+        <v>35305820</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -2149,7 +2149,7 @@
         <v>16080585</v>
       </c>
       <c r="C28">
-        <v>16143443</v>
+        <v>34554925</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -2160,7 +2160,7 @@
         <v>17970816</v>
       </c>
       <c r="C29">
-        <v>18357767</v>
+        <v>34137404</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -2171,7 +2171,7 @@
         <v>20021373</v>
       </c>
       <c r="C30">
-        <v>20416740</v>
+        <v>34632744</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -2182,7 +2182,7 @@
         <v>21643976</v>
       </c>
       <c r="C31">
-        <v>21731780</v>
+        <v>34763739</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -2193,7 +2193,7 @@
         <v>24399262</v>
       </c>
       <c r="C32">
-        <v>24304082</v>
+        <v>34131775</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -2204,7 +2204,7 @@
         <v>26853803</v>
       </c>
       <c r="C33">
-        <v>26939399</v>
+        <v>34729742</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -2215,7 +2215,7 @@
         <v>29383052</v>
       </c>
       <c r="C34">
-        <v>29492673</v>
+        <v>34495461</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -2226,7 +2226,7 @@
         <v>31968702</v>
       </c>
       <c r="C35">
-        <v>32112793</v>
+        <v>35604467</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -2237,7 +2237,7 @@
         <v>34530146</v>
       </c>
       <c r="C36">
-        <v>34327158</v>
+        <v>37001781</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -2248,7 +2248,7 @@
         <v>38158970</v>
       </c>
       <c r="C37">
-        <v>38931702</v>
+        <v>35034148</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -2259,7 +2259,7 @@
         <v>41322603</v>
       </c>
       <c r="C38">
-        <v>40955109</v>
+        <v>34622546</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -2270,7 +2270,7 @@
         <v>44684355</v>
       </c>
       <c r="C39">
-        <v>44334295</v>
+        <v>34796305</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -2281,7 +2281,7 @@
         <v>48450923</v>
       </c>
       <c r="C40">
-        <v>46776635</v>
+        <v>34311252</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -2292,7 +2292,7 @@
         <v>50170887</v>
       </c>
       <c r="C41">
-        <v>49583174</v>
+        <v>35468807</v>
       </c>
     </row>
   </sheetData>
@@ -2310,8 +2310,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2:R6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>